<commit_message>
ad status code to excel
</commit_message>
<xml_diff>
--- a/TestData/ProductRules.xlsx
+++ b/TestData/ProductRules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tokyomanamela/git/APIAutomation/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B540145-FAF3-EE48-A6ED-37EC3A177E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B67FD64-A07E-F649-BFFA-BB18C63FCF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1500" windowWidth="27240" windowHeight="15440" activeTab="1" xr2:uid="{47FBA647-1868-6E40-A4C7-16956C1A9E32}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>Mainlife_maxAge</t>
+  </si>
+  <si>
+    <t>StatusCode</t>
   </si>
 </sst>
 </file>
@@ -634,346 +637,355 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11926FA2-04CA-714C-8512-F4DE610ACF08}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="27.83203125" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" customWidth="1"/>
-    <col min="12" max="12" width="34" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" customWidth="1"/>
-    <col min="16" max="16" width="25.5" customWidth="1"/>
-    <col min="17" max="17" width="22.6640625" customWidth="1"/>
-    <col min="18" max="19" width="17.5" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1"/>
-    <col min="21" max="21" width="18.83203125" customWidth="1"/>
-    <col min="22" max="22" width="17.83203125" customWidth="1"/>
-    <col min="23" max="23" width="21.33203125" customWidth="1"/>
-    <col min="24" max="24" width="22" customWidth="1"/>
-    <col min="25" max="26" width="14.83203125" customWidth="1"/>
-    <col min="27" max="27" width="23.6640625" customWidth="1"/>
-    <col min="28" max="28" width="18" customWidth="1"/>
-    <col min="29" max="29" width="22" customWidth="1"/>
-    <col min="30" max="31" width="25.83203125" customWidth="1"/>
-    <col min="32" max="32" width="15.6640625" customWidth="1"/>
-    <col min="33" max="33" width="16.5" customWidth="1"/>
+    <col min="1" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" customWidth="1"/>
+    <col min="13" max="13" width="34" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" customWidth="1"/>
+    <col min="17" max="17" width="25.5" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" customWidth="1"/>
+    <col min="19" max="20" width="17.5" customWidth="1"/>
+    <col min="21" max="21" width="19.33203125" customWidth="1"/>
+    <col min="22" max="22" width="18.83203125" customWidth="1"/>
+    <col min="23" max="23" width="17.83203125" customWidth="1"/>
+    <col min="24" max="24" width="21.33203125" customWidth="1"/>
+    <col min="25" max="25" width="22" customWidth="1"/>
+    <col min="26" max="27" width="14.83203125" customWidth="1"/>
+    <col min="28" max="28" width="23.6640625" customWidth="1"/>
+    <col min="29" max="29" width="18" customWidth="1"/>
+    <col min="30" max="30" width="22" customWidth="1"/>
+    <col min="31" max="32" width="25.83203125" customWidth="1"/>
+    <col min="33" max="33" width="15.6640625" customWidth="1"/>
+    <col min="34" max="34" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
+        <v>200</v>
+      </c>
+      <c r="C2" s="2">
         <v>60100000</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
       <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
         <v>10000</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>50000</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>18</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>79</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>0</v>
       </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
       <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
         <v>10000</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>50000</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>18</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>79</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" s="5">
+      <c r="V2" s="5">
         <v>0</v>
       </c>
-      <c r="V2" s="5">
+      <c r="W2" s="5">
         <v>5</v>
       </c>
-      <c r="W2" s="5">
+      <c r="X2" s="5">
         <v>5000</v>
       </c>
-      <c r="X2" s="5">
+      <c r="Y2" s="5">
         <v>20000</v>
       </c>
-      <c r="Y2" s="5">
+      <c r="Z2" s="5">
         <v>0</v>
       </c>
-      <c r="Z2" s="5">
+      <c r="AA2" s="5">
         <v>18</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" s="5">
-        <v>1</v>
-      </c>
       <c r="AC2" s="5">
         <v>1</v>
       </c>
       <c r="AD2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="5">
         <v>10000</v>
       </c>
-      <c r="AE2" s="5">
+      <c r="AF2" s="5">
         <v>20000</v>
       </c>
-      <c r="AF2" s="5">
+      <c r="AG2" s="5">
         <v>18</v>
       </c>
-      <c r="AG2" s="5">
+      <c r="AH2" s="5">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
+        <v>200</v>
+      </c>
+      <c r="C3" s="2">
         <v>60200000</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
       <c r="H3" s="2">
         <v>1</v>
       </c>
       <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
         <v>10000</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>50000</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>18</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>79</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>0</v>
       </c>
-      <c r="O3" s="2">
-        <v>1</v>
-      </c>
       <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
         <v>10000</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>50000</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>18</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>79</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U3" s="5">
+      <c r="V3" s="5">
         <v>0</v>
       </c>
-      <c r="V3" s="5">
+      <c r="W3" s="5">
         <v>5</v>
       </c>
-      <c r="W3" s="5">
+      <c r="X3" s="5">
         <v>5000</v>
       </c>
-      <c r="X3" s="5">
+      <c r="Y3" s="5">
         <v>20000</v>
       </c>
-      <c r="Y3" s="5">
+      <c r="Z3" s="5">
         <v>0</v>
       </c>
-      <c r="Z3" s="5">
+      <c r="AA3" s="5">
         <v>18</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AB3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AB3" s="5">
-        <v>1</v>
-      </c>
       <c r="AC3" s="5">
         <v>1</v>
       </c>
       <c r="AD3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="5">
         <v>10000</v>
       </c>
-      <c r="AE3" s="5">
+      <c r="AF3" s="5">
         <v>20000</v>
       </c>
-      <c r="AF3" s="5">
+      <c r="AG3" s="5">
         <v>18</v>
       </c>
-      <c r="AG3" s="5">
+      <c r="AH3" s="5">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Errors fixed and updated
</commit_message>
<xml_diff>
--- a/TestData/ProductRules.xlsx
+++ b/TestData/ProductRules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tokyomanamela/git/APIAutomation/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thaboramalitse/git/APIAutomation/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66F0529-D3B6-C848-A475-B6B554403E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906D1163-1E0C-D543-B318-0E898D477800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1400" windowWidth="27240" windowHeight="15440" xr2:uid="{47FBA647-1868-6E40-A4C7-16956C1A9E32}"/>
+    <workbookView xWindow="1020" yWindow="1400" windowWidth="27240" windowHeight="15440" activeTab="1" xr2:uid="{47FBA647-1868-6E40-A4C7-16956C1A9E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Request" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>Elite V6.0</t>
+  </si>
+  <si>
+    <t>Core V6.0</t>
+  </si>
+  <si>
+    <t>Lite V6.0</t>
   </si>
 </sst>
 </file>
@@ -615,7 +621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB08A70C-F7ED-4747-8773-33F8D74C707E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -762,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11926FA2-04CA-714C-8512-F4DE610ACF08}">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1212,7 @@
         <v>10</v>
       </c>
       <c r="X5" s="2">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="Y5" s="2">
         <v>50000</v>
@@ -1250,7 +1256,7 @@
         <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
         <v>46</v>
@@ -1277,7 +1283,7 @@
         <v>18</v>
       </c>
       <c r="M6" s="2">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="N6" t="s">
         <v>31</v>
@@ -1354,7 +1360,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
renamed test data file
</commit_message>
<xml_diff>
--- a/TestData/ProductRules.xlsx
+++ b/TestData/ProductRules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thaboramalitse/git/APIAutomation/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tokyomanamela/git/APIAutomation/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906D1163-1E0C-D543-B318-0E898D477800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F845C227-FC7C-4844-BDDB-BFC0854A8DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1400" windowWidth="27240" windowHeight="15440" activeTab="1" xr2:uid="{47FBA647-1868-6E40-A4C7-16956C1A9E32}"/>
+    <workbookView xWindow="300" yWindow="720" windowWidth="27240" windowHeight="15440" activeTab="1" xr2:uid="{47FBA647-1868-6E40-A4C7-16956C1A9E32}"/>
   </bookViews>
   <sheets>
     <sheet name="Request" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -46,9 +46,6 @@
     <t>ProductCode</t>
   </si>
   <si>
-    <t>TC_001_60100000</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -172,42 +169,18 @@
     <t>StatusCode</t>
   </si>
   <si>
-    <t>TC_002_60200000</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>TC_003_1975</t>
-  </si>
-  <si>
-    <t>TC_004_1960E</t>
-  </si>
-  <si>
     <t>1960E</t>
   </si>
   <si>
-    <t>TC_005_1960C</t>
-  </si>
-  <si>
     <t>1960C</t>
   </si>
   <si>
-    <t>TC_006_1960L</t>
-  </si>
-  <si>
     <t>1960L</t>
   </si>
   <si>
-    <t>TC_007_1977</t>
-  </si>
-  <si>
-    <t>TC_008_1924</t>
-  </si>
-  <si>
-    <t>Getting product rule for 1975</t>
-  </si>
-  <si>
     <t>Getting product rule for Elite V6.0</t>
   </si>
   <si>
@@ -221,6 +194,42 @@
   </si>
   <si>
     <t>Lite V6.0</t>
+  </si>
+  <si>
+    <t>Getting product rule for  product 1975</t>
+  </si>
+  <si>
+    <t>Getting product rule for Core V6.0</t>
+  </si>
+  <si>
+    <t>Getting product rule for Lite V6.0</t>
+  </si>
+  <si>
+    <t>Getting product rule for Elite V6.0(Product 1924)</t>
+  </si>
+  <si>
+    <t>TC _001_ProductRules_60100000</t>
+  </si>
+  <si>
+    <t>TC _002_ProductRules_60200000</t>
+  </si>
+  <si>
+    <t>TC _003_ProductRules_1975</t>
+  </si>
+  <si>
+    <t>TC _004_ProductRules_1960E</t>
+  </si>
+  <si>
+    <t>TC _005_ProductRules_1960C</t>
+  </si>
+  <si>
+    <t>TC _006_ProductRules_1960L</t>
+  </si>
+  <si>
+    <t>TC _007_ProductRules_1977</t>
+  </si>
+  <si>
+    <t>TC  _008_ProductRules_1924</t>
   </si>
 </sst>
 </file>
@@ -622,14 +631,14 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="43.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -641,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -649,13 +658,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>60100000</v>
@@ -663,13 +672,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>60200000</v>
@@ -677,13 +686,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D4" s="2">
         <v>1975</v>
@@ -691,55 +700,55 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2">
         <v>1977</v>
@@ -747,13 +756,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2">
         <v>1924</v>
@@ -769,12 +778,13 @@
   <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="22.1640625" customWidth="1"/>
@@ -811,108 +821,108 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2">
         <v>200</v>
@@ -921,16 +931,16 @@
         <v>60100000</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -951,7 +961,7 @@
         <v>79</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -972,7 +982,7 @@
         <v>79</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V2" s="5">
         <v>0</v>
@@ -993,7 +1003,7 @@
         <v>20</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC2" s="5">
         <v>0</v>
@@ -1016,7 +1026,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2">
         <v>200</v>
@@ -1025,16 +1035,16 @@
         <v>60200000</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -1055,7 +1065,7 @@
         <v>79</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O3" s="2">
         <v>0</v>
@@ -1076,7 +1086,7 @@
         <v>79</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V3" s="5">
         <v>0</v>
@@ -1097,7 +1107,7 @@
         <v>20</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC3" s="5">
         <v>0</v>
@@ -1120,7 +1130,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2">
         <v>200</v>
@@ -1129,7 +1139,7 @@
         <v>1975</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -1143,25 +1153,25 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2">
         <v>200</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
@@ -1182,7 +1192,7 @@
         <v>59</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O5" s="2">
         <v>0</v>
@@ -1203,7 +1213,7 @@
         <v>75</v>
       </c>
       <c r="U5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V5" s="2">
         <v>0</v>
@@ -1224,7 +1234,7 @@
         <v>20</v>
       </c>
       <c r="AB5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC5" s="2">
         <v>0</v>
@@ -1247,25 +1257,25 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2">
         <v>200</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" t="s">
-        <v>60</v>
-      </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
@@ -1286,7 +1296,7 @@
         <v>75</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
@@ -1307,7 +1317,7 @@
         <v>75</v>
       </c>
       <c r="U6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V6" s="2">
         <v>0</v>
@@ -1328,7 +1338,7 @@
         <v>20</v>
       </c>
       <c r="AB6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC6" s="2">
         <v>0</v>
@@ -1351,25 +1361,25 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2">
         <v>200</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -1390,7 +1400,7 @@
         <v>75</v>
       </c>
       <c r="N7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O7" s="2">
         <v>0</v>
@@ -1411,7 +1421,7 @@
         <v>75</v>
       </c>
       <c r="U7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V7" s="2">
         <v>0</v>
@@ -1432,7 +1442,7 @@
         <v>20</v>
       </c>
       <c r="AB7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC7" s="2">
         <v>0</v>
@@ -1455,7 +1465,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2">
         <v>200</v>
@@ -1464,7 +1474,7 @@
         <v>1977</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
@@ -1478,7 +1488,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B9" s="2">
         <v>200</v>
@@ -1487,10 +1497,10 @@
         <v>1924</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>

</xml_diff>